<commit_message>
Ponerle colorcito a la solución de la tabla
</commit_message>
<xml_diff>
--- a/BorgesCano.Adrian_GonzalezMartinez.Marco_PL4/Problema3Tema4.xlsx
+++ b/BorgesCano.Adrian_GonzalezMartinez.Marco_PL4/Problema3Tema4.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CosasUni\AYC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adriii.bc/Documents/GitHub/BorgesCano.Adrian_GonzalezMartinez.Marco_PL4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8ECAA5-A295-4DB5-897A-7EF9ABE34247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2446CF-12AE-6D4E-9E95-C5CD13877BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3C89C0BD-12A6-4EB9-ADB6-2AB09CE808EE}"/>
+    <workbookView xWindow="44900" yWindow="7440" windowWidth="33320" windowHeight="17700" xr2:uid="{3C89C0BD-12A6-4EB9-ADB6-2AB09CE808EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -189,12 +188,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -209,12 +226,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,19 +558,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430659B3-1A09-4EBD-8671-AA2284137861}">
   <dimension ref="B1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="15" width="13.33203125" customWidth="1"/>
     <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.2">
       <c r="H1">
         <v>0</v>
       </c>
@@ -554,50 +584,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
         <v>11</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3">
         <v>1</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="3">
         <v>2</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="3">
         <v>3</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="3">
         <v>4</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="3">
         <v>5</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="3">
         <v>6</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="3">
         <v>7</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="3">
         <v>8</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="3">
         <v>9</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="Q2" s="3">
         <v>10</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="3">
         <v>11</v>
       </c>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -610,7 +640,7 @@
       <c r="E3">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -647,7 +677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -660,7 +690,7 @@
       <c r="E4">
         <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -697,48 +727,48 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="G5" t="s">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="G5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -752,7 +782,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -766,7 +796,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -780,7 +810,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -793,7 +823,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
       <c r="G13" t="s">
         <v>33</v>
       </c>
@@ -804,7 +834,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
       <c r="G14" t="s">
         <v>34</v>
       </c>
@@ -815,7 +845,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F19" t="s">
         <v>42</v>
       </c>
@@ -826,7 +856,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F20" t="s">
         <v>43</v>
       </c>

</xml_diff>